<commit_message>
Fixed some errors in labeling of files.
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint 2/Sprint 2 BurndownChart.xlsx
+++ b/Project/Phase 2/Sprint 2/Sprint 2 BurndownChart.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruna Arroja\Documents\Faculdade\3ºAno\1ºSemestre\ES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\IdeaProjects\jabref\Project\Phase 2\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD77716F-2689-4C98-BA00-90BCB7246EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -74,16 +75,16 @@
     <t>Day 7</t>
   </si>
   <si>
-    <t>User storie</t>
+    <t>Planning</t>
   </si>
   <si>
-    <t>Planning</t>
+    <t>User story</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\-d"/>
   </numFmts>
@@ -414,9 +415,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -453,7 +454,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -594,7 +594,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7EC3-4EA3-B9DF-582245A3220D}"/>
             </c:ext>
@@ -695,7 +695,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7EC3-4EA3-B9DF-582245A3220D}"/>
             </c:ext>
@@ -830,7 +830,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -862,14 +861,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1480,7 +1479,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6A6B446-ED28-4837-A2F6-260D1C27ED32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6A6B446-ED28-4837-A2F6-260D1C27ED32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1698,23 +1697,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B2:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="72.44140625" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="72.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
@@ -1729,7 +1728,7 @@
       <c r="K2" s="37"/>
       <c r="L2" s="23"/>
     </row>
-    <row r="3" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1740,7 +1739,7 @@
       <c r="I3" s="1"/>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="30" t="s">
         <v>1</v>
       </c>
@@ -1773,7 +1772,7 @@
       </c>
       <c r="L4" s="16"/>
     </row>
-    <row r="5" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
       <c r="D5" s="7" t="s">
@@ -1802,12 +1801,12 @@
       </c>
       <c r="L5" s="17"/>
     </row>
-    <row r="6" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="11">
         <v>40</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="8">
         <v>1</v>
@@ -1835,12 +1834,12 @@
       </c>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="11">
         <v>41</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="8">
         <v>7</v>
@@ -1868,7 +1867,7 @@
       </c>
       <c r="L7" s="18"/>
     </row>
-    <row r="8" spans="2:12" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" s="24"/>
       <c r="C8" s="25"/>
       <c r="D8" s="20"/>
@@ -1881,7 +1880,7 @@
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
     </row>
-    <row r="9" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="24"/>
       <c r="C9" s="25"/>
       <c r="D9" s="20"/>
@@ -1894,7 +1893,7 @@
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
     </row>
-    <row r="10" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="24"/>
       <c r="C10" s="25"/>
       <c r="D10" s="20"/>
@@ -1907,7 +1906,7 @@
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
     </row>
-    <row r="11" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="24"/>
       <c r="C11" s="25"/>
       <c r="D11" s="20"/>
@@ -1920,7 +1919,7 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
     </row>
-    <row r="12" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="24"/>
       <c r="C12" s="25"/>
       <c r="D12" s="20"/>
@@ -1933,7 +1932,7 @@
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
     </row>
-    <row r="13" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="24"/>
       <c r="C13" s="25"/>
       <c r="D13" s="20"/>
@@ -1946,7 +1945,7 @@
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="24"/>
       <c r="C14" s="25"/>
       <c r="D14" s="20"/>
@@ -1959,7 +1958,7 @@
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
     </row>
-    <row r="15" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="24"/>
       <c r="C15" s="25"/>
       <c r="D15" s="20"/>
@@ -1972,7 +1971,7 @@
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
     </row>
-    <row r="16" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="24"/>
       <c r="C16" s="25"/>
       <c r="D16" s="20"/>
@@ -1985,7 +1984,7 @@
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="24"/>
       <c r="C17" s="25"/>
       <c r="D17" s="20"/>
@@ -1998,7 +1997,7 @@
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="24"/>
       <c r="C18" s="25"/>
       <c r="D18" s="20"/>
@@ -2011,7 +2010,7 @@
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="24"/>
       <c r="C19" s="25"/>
       <c r="D19" s="20"/>
@@ -2024,7 +2023,7 @@
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="24"/>
       <c r="C20" s="25"/>
       <c r="D20" s="20"/>
@@ -2037,7 +2036,7 @@
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="24"/>
       <c r="C21" s="25"/>
       <c r="D21" s="20"/>
@@ -2050,7 +2049,7 @@
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="20"/>
       <c r="C22" s="26"/>
       <c r="D22" s="20"/>
@@ -2063,7 +2062,7 @@
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="28"/>
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
@@ -2076,7 +2075,7 @@
       <c r="K23" s="29"/>
       <c r="L23" s="19"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="32" t="s">
         <v>10</v>
       </c>
@@ -2086,36 +2085,36 @@
         <v>8</v>
       </c>
       <c r="E24" s="27">
-        <f>D24-SUM(E6:E7)</f>
+        <f t="shared" ref="E24:K24" si="0">D24-SUM(E6:E7)</f>
         <v>6</v>
       </c>
       <c r="F24" s="27">
-        <f>E24-SUM(F6:F7)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G24" s="27">
-        <f>F24-SUM(G6:G7)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H24" s="27">
-        <f>G24-SUM(H6:H7)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I24" s="27">
-        <f>H24-SUM(I6:I7)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J24" s="27">
-        <f>I24-SUM(J6:J7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K24" s="27">
-        <f>J24-SUM(K6:K7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L24" s="20"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="34" t="s">
         <v>11</v>
       </c>
@@ -2154,7 +2153,7 @@
       </c>
       <c r="L25" s="20"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -2165,7 +2164,7 @@
       <c r="I26" s="13"/>
       <c r="L26" s="15"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -2175,7 +2174,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -2185,7 +2184,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -2195,7 +2194,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
@@ -2205,7 +2204,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="4"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -2215,7 +2214,7 @@
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -2225,7 +2224,7 @@
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="4"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2235,7 +2234,7 @@
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -2245,7 +2244,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
@@ -2255,7 +2254,7 @@
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
@@ -2265,7 +2264,7 @@
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
@@ -2275,7 +2274,7 @@
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
@@ -2285,7 +2284,7 @@
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="4"/>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
@@ -2295,7 +2294,7 @@
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
@@ -2305,7 +2304,7 @@
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
@@ -2315,7 +2314,7 @@
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
@@ -2325,7 +2324,7 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="4"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
@@ -2335,7 +2334,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="4"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>

</xml_diff>